<commit_message>
Objectif 1 avec nvx deltas
</commit_message>
<xml_diff>
--- a/par_p_par_c/delta_tables.xlsx
+++ b/par_p_par_c/delta_tables.xlsx
@@ -730,10 +730,10 @@
         <v>-0.19</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.21</v>
+        <v>-0.22</v>
       </c>
       <c r="F4" t="n">
-        <v>-0</v>
+        <v>-0.01</v>
       </c>
       <c r="G4" t="n">
         <v>0.66</v>
@@ -742,7 +742,7 @@
         <v>-0.43</v>
       </c>
       <c r="I4" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="J4" t="n">
         <v>-4.39</v>
@@ -835,7 +835,7 @@
         <v>-0.52</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H5" t="n">
         <v>-0.31</v>
@@ -935,7 +935,7 @@
         <v>-0.58</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.61</v>
+        <v>-0.62</v>
       </c>
       <c r="G6" t="n">
         <v>-0.11</v>
@@ -1137,7 +1137,7 @@
         <v>0.33</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
       <c r="G8" t="n">
         <v>-0.03</v>
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="E9" t="n">
         <v>0.22</v>
@@ -1578,10 +1578,10 @@
       </c>
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>-0.21</v>
+        <v>-0.23</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4500000000000001</v>
+        <v>0.43</v>
       </c>
       <c r="F4" t="n">
         <v>-0.24</v>
@@ -1620,7 +1620,7 @@
         <v>-0.79</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.6900000000000001</v>
+        <v>-0.7000000000000001</v>
       </c>
       <c r="F5" t="n">
         <v>-0.28</v>
@@ -1660,10 +1660,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-1.19</v>
+        <v>-1.2</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.3</v>
+        <v>-1.31</v>
       </c>
       <c r="F6" t="n">
         <v>-0.5600000000000001</v>
@@ -1742,10 +1742,10 @@
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
       <c r="E8" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="F8" t="n">
         <v>-0.11</v>

</xml_diff>

<commit_message>
Ajout de ['Basal'] par_p_par_c
</commit_message>
<xml_diff>
--- a/par_p_par_c/delta_tables.xlsx
+++ b/par_p_par_c/delta_tables.xlsx
@@ -529,7 +529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG15"/>
+  <dimension ref="A1:AL15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,29 +541,29 @@
     <col width="15.6" customWidth="1" min="2" max="2"/>
     <col width="14.4" customWidth="1" min="3" max="3"/>
     <col width="8.4" customWidth="1" min="4" max="4"/>
-    <col width="13.2" customWidth="1" min="5" max="5"/>
-    <col width="9.6" customWidth="1" min="6" max="6"/>
-    <col width="8.4" customWidth="1" min="7" max="7"/>
+    <col width="8.4" customWidth="1" min="5" max="5"/>
+    <col width="13.2" customWidth="1" min="6" max="6"/>
+    <col width="9.6" customWidth="1" min="7" max="7"/>
     <col width="8.4" customWidth="1" min="8" max="8"/>
     <col width="8.4" customWidth="1" min="9" max="9"/>
     <col width="8.4" customWidth="1" min="10" max="10"/>
-    <col width="13.2" customWidth="1" min="11" max="11"/>
-    <col width="9.6" customWidth="1" min="12" max="12"/>
-    <col width="8.4" customWidth="1" min="13" max="13"/>
-    <col width="8.4" customWidth="1" min="14" max="14"/>
+    <col width="9.6" customWidth="1" min="11" max="11"/>
+    <col width="8.4" customWidth="1" min="12" max="12"/>
+    <col width="13.2" customWidth="1" min="13" max="13"/>
+    <col width="9.6" customWidth="1" min="14" max="14"/>
     <col width="8.4" customWidth="1" min="15" max="15"/>
-    <col width="9.6" customWidth="1" min="16" max="16"/>
-    <col width="13.2" customWidth="1" min="17" max="17"/>
+    <col width="8.4" customWidth="1" min="16" max="16"/>
+    <col width="8.4" customWidth="1" min="17" max="17"/>
     <col width="9.6" customWidth="1" min="18" max="18"/>
-    <col width="8.4" customWidth="1" min="19" max="19"/>
-    <col width="8.4" customWidth="1" min="20" max="20"/>
+    <col width="9.6" customWidth="1" min="19" max="19"/>
+    <col width="13.2" customWidth="1" min="20" max="20"/>
     <col width="9.6" customWidth="1" min="21" max="21"/>
     <col width="8.4" customWidth="1" min="22" max="22"/>
-    <col width="13.2" customWidth="1" min="23" max="23"/>
+    <col width="8.4" customWidth="1" min="23" max="23"/>
     <col width="9.6" customWidth="1" min="24" max="24"/>
-    <col width="8.4" customWidth="1" min="25" max="25"/>
+    <col width="9.6" customWidth="1" min="25" max="25"/>
     <col width="8.4" customWidth="1" min="26" max="26"/>
-    <col width="13.2" customWidth="1" min="28" max="28"/>
+    <col width="12" customWidth="1" min="32" max="32"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -584,46 +584,51 @@
       <c r="G1" s="2" t="n"/>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>PD</t>
         </is>
       </c>
-      <c r="K1" s="2" t="n"/>
       <c r="L1" s="2" t="n"/>
       <c r="M1" s="2" t="n"/>
       <c r="N1" s="2" t="n"/>
       <c r="O1" s="2" t="n"/>
-      <c r="P1" s="6" t="inlineStr">
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="6" t="inlineStr">
         <is>
           <t>Ieq</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
       <c r="S1" s="2" t="n"/>
       <c r="T1" s="2" t="n"/>
       <c r="U1" s="2" t="n"/>
-      <c r="V1" s="7" t="inlineStr">
-        <is>
-          <t>Iraw</t>
-        </is>
-      </c>
+      <c r="V1" s="2" t="n"/>
       <c r="W1" s="2" t="n"/>
       <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
+      <c r="Y1" s="7" t="inlineStr">
+        <is>
+          <t>Iraw</t>
+        </is>
+      </c>
       <c r="Z1" s="2" t="n"/>
       <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="8" t="inlineStr">
-        <is>
-          <t>RT</t>
-        </is>
-      </c>
+      <c r="AB1" s="2" t="n"/>
       <c r="AC1" s="2" t="n"/>
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="2" t="n"/>
-      <c r="AF1" s="2" t="n"/>
+      <c r="AF1" s="8" t="inlineStr">
+        <is>
+          <t>RT</t>
+        </is>
+      </c>
       <c r="AG1" s="2" t="n"/>
+      <c r="AH1" s="2" t="n"/>
+      <c r="AI1" s="2" t="n"/>
+      <c r="AJ1" s="2" t="n"/>
+      <c r="AK1" s="2" t="n"/>
+      <c r="AL1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="C2" s="1" t="inlineStr">
@@ -633,150 +638,175 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
+          <t>Basal</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
           <t>ΔAmi</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>ΔFsk/IBMX</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>ΔVX770</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>ΔApi</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>ΔInh</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>ΔATP</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>Basal</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>ΔAmi</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>ΔFsk/IBMX</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>ΔVX770</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>ΔApi</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>ΔInh</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>ΔATP</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>Basal</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>ΔAmi</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>ΔFsk/IBMX</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>ΔVX770</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>ΔApi</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>ΔInh</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>ΔATP</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
+        <is>
+          <t>Basal</t>
+        </is>
+      </c>
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>ΔAmi</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>ΔFsk/IBMX</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>ΔVX770</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
         <is>
           <t>ΔApi</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
+      <c r="AD2" s="1" t="inlineStr">
         <is>
           <t>ΔInh</t>
         </is>
       </c>
-      <c r="AA2" s="1" t="inlineStr">
+      <c r="AE2" s="1" t="inlineStr">
         <is>
           <t>ΔATP</t>
         </is>
       </c>
-      <c r="AB2" s="1" t="inlineStr">
+      <c r="AF2" s="1" t="inlineStr">
+        <is>
+          <t>Basal</t>
+        </is>
+      </c>
+      <c r="AG2" s="1" t="inlineStr">
         <is>
           <t>ΔAmi</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
+      <c r="AH2" s="1" t="inlineStr">
         <is>
           <t>ΔFsk/IBMX</t>
         </is>
       </c>
-      <c r="AD2" s="1" t="inlineStr">
+      <c r="AI2" s="1" t="inlineStr">
         <is>
           <t>ΔVX770</t>
         </is>
       </c>
-      <c r="AE2" s="1" t="inlineStr">
+      <c r="AJ2" s="1" t="inlineStr">
         <is>
           <t>ΔApi</t>
         </is>
       </c>
-      <c r="AF2" s="1" t="inlineStr">
+      <c r="AK2" s="1" t="inlineStr">
         <is>
           <t>ΔInh</t>
         </is>
       </c>
-      <c r="AG2" s="1" t="inlineStr">
+      <c r="AL2" s="1" t="inlineStr">
         <is>
           <t>ΔATP</t>
         </is>
@@ -810,221 +840,247 @@
           <t>ctrl</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>vx770</t>
-        </is>
-      </c>
+      <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" t="n">
+        <v>13.35</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.01</v>
       </c>
-      <c r="E4" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-0.13</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>-0.06</v>
       </c>
-      <c r="H4" t="n">
+      <c r="K4" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-3.54</v>
+      </c>
+      <c r="M4" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="J4" t="n">
-        <v>-1.59</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.18</v>
-      </c>
       <c r="N4" t="n">
-        <v>-0.41</v>
+        <v>0.1</v>
       </c>
       <c r="O4" t="n">
-        <v>0.67</v>
+        <v>-0.01</v>
       </c>
       <c r="P4" t="n">
-        <v>22.92</v>
+        <v>0.1</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.32</v>
+        <v>-0.2</v>
       </c>
       <c r="R4" t="n">
-        <v>-8.33</v>
+        <v>-47.95</v>
       </c>
       <c r="S4" t="n">
-        <v>-2.81</v>
+        <v>48.6</v>
       </c>
       <c r="T4" t="n">
-        <v>6.38</v>
+        <v>-0.27</v>
       </c>
       <c r="U4" t="n">
-        <v>-10.09</v>
+        <v>-1.44</v>
       </c>
       <c r="V4" t="n">
-        <v>19.76</v>
+        <v>1.04</v>
       </c>
       <c r="W4" t="n">
-        <v>20.58</v>
+        <v>-2.21</v>
       </c>
       <c r="X4" t="n">
-        <v>10.61</v>
+        <v>2.78</v>
       </c>
       <c r="Y4" t="n">
-        <v>7.14</v>
+        <v>2.35</v>
       </c>
       <c r="Z4" t="n">
-        <v>13.66</v>
+        <v>-0.16</v>
       </c>
       <c r="AA4" t="n">
-        <v>3.09</v>
+        <v>0.26</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.04</v>
+        <v>-0.78</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.33</v>
+        <v>0.48</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.55</v>
+        <v>-1.43</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.24</v>
+        <v>1.68</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.01</v>
+        <v>79.34999999999999</v>
       </c>
       <c r="AG4" t="n">
-        <v>-0.1</v>
+        <v>-0.26</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="n"/>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>vx661-vx445</t>
-        </is>
-      </c>
+      <c r="B5" s="10" t="n"/>
       <c r="C5" s="1" t="inlineStr">
         <is>
           <t>vx770</t>
         </is>
       </c>
       <c r="D5" t="n">
+        <v>15.49</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.13</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.03</v>
       </c>
-      <c r="E5" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.13</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="H5" t="n">
+      <c r="K5" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1.59</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-0.41</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-7.88</v>
+      </c>
+      <c r="S5" t="n">
+        <v>22.92</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-8.33</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-2.81</v>
+      </c>
+      <c r="W5" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-10.09</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-59.67</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>19.76</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>20.58</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>10.61</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>7.14</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>13.66</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>64.59</v>
+      </c>
+      <c r="AG5" t="n">
         <v>-0.04</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-0.11</v>
-      </c>
-      <c r="P5" t="n">
-        <v>-2.51</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>-0.73</v>
-      </c>
-      <c r="R5" t="n">
-        <v>-2.98</v>
-      </c>
-      <c r="S5" t="n">
-        <v>-1.03</v>
-      </c>
-      <c r="T5" t="n">
-        <v>-0.11</v>
-      </c>
-      <c r="U5" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="V5" t="n">
-        <v>7.33</v>
-      </c>
-      <c r="W5" t="n">
-        <v>6.24</v>
-      </c>
-      <c r="X5" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>2.27</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>-0.14</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>-0.08</v>
+      <c r="AH5" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>ctrl</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr"/>
+          <t>vx661-vx445</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>vx770</t>
+        </is>
+      </c>
       <c r="D6" t="n">
-        <v>0.06</v>
+        <v>14.26</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.04</v>
+        <v>0.03</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.23</v>
+        <v>-0.06</v>
       </c>
       <c r="G6" t="n">
         <v>-0.13</v>
@@ -1033,181 +1089,207 @@
         <v>-0.06</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.02</v>
+        <v>-0.04</v>
       </c>
       <c r="J6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="R6" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-2.51</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-0.73</v>
+      </c>
+      <c r="U6" t="n">
         <v>-2.98</v>
       </c>
-      <c r="K6" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="N6" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="P6" t="n">
-        <v>30.17</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="R6" t="n">
-        <v>-1.55</v>
-      </c>
-      <c r="S6" t="n">
-        <v>-0.37</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.27</v>
-      </c>
       <c r="V6" t="n">
-        <v>-0.93</v>
+        <v>-1.03</v>
       </c>
       <c r="W6" t="n">
-        <v>2.08</v>
+        <v>-0.11</v>
       </c>
       <c r="X6" t="n">
-        <v>0.6</v>
+        <v>1.52</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.58</v>
+        <v>-48.84</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.64</v>
+        <v>7.33</v>
       </c>
       <c r="AA6" t="n">
-        <v>2.21</v>
+        <v>6.24</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.53</v>
+        <v>2.22</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.34</v>
+        <v>0.92</v>
       </c>
       <c r="AD6" t="n">
-        <v>2.22</v>
+        <v>1.1</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.38</v>
+        <v>2.27</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.6</v>
+        <v>70.7</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.24</v>
+        <v>-0.14</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>-0.08</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n"/>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>vx661-vx445</t>
-        </is>
-      </c>
+      <c r="B7" s="10" t="n"/>
       <c r="C7" s="1" t="inlineStr">
         <is>
           <t>vx770-Api</t>
         </is>
       </c>
       <c r="D7" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.01</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>-0.12</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>-0.15</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>-0.16</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>-0.14</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.05</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="L7" t="n">
         <v>-6.26</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>-0.12</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>0.54</v>
       </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>0.13</v>
       </c>
-      <c r="N7" t="n">
+      <c r="P7" t="n">
         <v>0</v>
       </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
         <v>0.2</v>
       </c>
-      <c r="P7" t="n">
+      <c r="R7" t="n">
+        <v>-70.75</v>
+      </c>
+      <c r="S7" t="n">
         <v>83.29000000000001</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="T7" t="n">
         <v>1.64</v>
       </c>
-      <c r="R7" t="n">
+      <c r="U7" t="n">
         <v>-7.2</v>
       </c>
-      <c r="S7" t="n">
+      <c r="V7" t="n">
         <v>-1.59</v>
       </c>
-      <c r="T7" t="n">
+      <c r="W7" t="n">
         <v>-0.55</v>
       </c>
-      <c r="U7" t="n">
+      <c r="X7" t="n">
         <v>-2.29</v>
       </c>
-      <c r="V7" t="n">
+      <c r="Y7" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="Z7" t="n">
         <v>14.58</v>
       </c>
-      <c r="W7" t="n">
+      <c r="AA7" t="n">
         <v>14.74</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AB7" t="n">
         <v>6.6</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AC7" t="n">
         <v>3.93</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AD7" t="n">
         <v>3.86</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AE7" t="n">
         <v>3.01</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AF7" t="n">
+        <v>75</v>
+      </c>
+      <c r="AG7" t="n">
         <v>-0.08</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AH7" t="n">
         <v>0.7</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AI7" t="n">
         <v>0.87</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AJ7" t="n">
         <v>0.97</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AK7" t="n">
         <v>0.87</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AL7" t="n">
         <v>-0.33</v>
       </c>
     </row>
@@ -1224,93 +1306,108 @@
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="E8" t="n">
         <v>-0.05</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>-0.04</v>
       </c>
-      <c r="F8" t="n">
-        <v>-0.07000000000000001</v>
-      </c>
       <c r="G8" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="H8" t="n">
         <v>-0.04</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>-0.15</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>0.04</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
+        <v>-6.4</v>
+      </c>
+      <c r="L8" t="n">
         <v>5.6</v>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
         <v>-0.06</v>
       </c>
-      <c r="L8" t="n">
+      <c r="N8" t="n">
         <v>0.02</v>
       </c>
-      <c r="M8" t="n">
+      <c r="O8" t="n">
         <v>0</v>
       </c>
-      <c r="N8" t="n">
+      <c r="P8" t="n">
         <v>0</v>
       </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
         <v>-0.58</v>
       </c>
-      <c r="P8" t="n">
+      <c r="R8" t="n">
+        <v>14.15</v>
+      </c>
+      <c r="S8" t="n">
         <v>-12.19</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="T8" t="n">
         <v>0.25</v>
       </c>
-      <c r="R8" t="n">
+      <c r="U8" t="n">
         <v>-0.15</v>
       </c>
-      <c r="S8" t="n">
+      <c r="V8" t="n">
         <v>-0.09</v>
       </c>
-      <c r="T8" t="n">
+      <c r="W8" t="n">
         <v>-0.11</v>
       </c>
-      <c r="U8" t="n">
+      <c r="X8" t="n">
         <v>1.1</v>
       </c>
-      <c r="V8" t="n">
+      <c r="Y8" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="Z8" t="n">
         <v>-2.41</v>
       </c>
-      <c r="W8" t="n">
+      <c r="AA8" t="n">
         <v>-0.05</v>
       </c>
-      <c r="X8" t="n">
+      <c r="AB8" t="n">
         <v>-0.26</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="AC8" t="n">
         <v>-0.33</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AD8" t="n">
         <v>-0.48</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AE8" t="n">
         <v>0.66</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AF8" t="n">
+        <v>428.49</v>
+      </c>
+      <c r="AG8" t="n">
         <v>6.45</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AH8" t="n">
         <v>7.19</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AI8" t="n">
         <v>12.63</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AJ8" t="n">
         <v>7.93</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AK8" t="n">
         <v>28.92</v>
       </c>
-      <c r="AG8" t="n">
+      <c r="AL8" t="n">
         <v>-9.99</v>
       </c>
     </row>
@@ -1323,93 +1420,108 @@
         </is>
       </c>
       <c r="D9" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="E9" t="n">
         <v>-0.09</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>-0.04</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>-0.13</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>-0.07000000000000001</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>-0.16</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>0.05</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
+        <v>-4.47</v>
+      </c>
+      <c r="L9" t="n">
         <v>3.19</v>
       </c>
-      <c r="K9" t="n">
+      <c r="M9" t="n">
         <v>-0.34</v>
       </c>
-      <c r="L9" t="n">
+      <c r="N9" t="n">
         <v>0.08</v>
       </c>
-      <c r="M9" t="n">
+      <c r="O9" t="n">
         <v>-0.11</v>
       </c>
-      <c r="N9" t="n">
+      <c r="P9" t="n">
         <v>0.1</v>
       </c>
-      <c r="O9" t="n">
+      <c r="Q9" t="n">
         <v>-0.2</v>
       </c>
-      <c r="P9" t="n">
+      <c r="R9" t="n">
+        <v>12.03</v>
+      </c>
+      <c r="S9" t="n">
         <v>-8.869999999999999</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="T9" t="n">
         <v>0.78</v>
       </c>
-      <c r="R9" t="n">
+      <c r="U9" t="n">
         <v>-0.39</v>
       </c>
-      <c r="S9" t="n">
+      <c r="V9" t="n">
         <v>0.11</v>
       </c>
-      <c r="T9" t="n">
+      <c r="W9" t="n">
         <v>-0.41</v>
       </c>
-      <c r="U9" t="n">
+      <c r="X9" t="n">
         <v>0.46</v>
       </c>
-      <c r="V9" t="n">
+      <c r="Y9" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="Z9" t="n">
         <v>-1.21</v>
       </c>
-      <c r="W9" t="n">
+      <c r="AA9" t="n">
         <v>1.17</v>
       </c>
-      <c r="X9" t="n">
+      <c r="AB9" t="n">
         <v>0.48</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AC9" t="n">
         <v>0.44</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AD9" t="n">
         <v>-0.18</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AE9" t="n">
         <v>0.7</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AF9" t="n">
+        <v>392.21</v>
+      </c>
+      <c r="AG9" t="n">
         <v>13.62</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AH9" t="n">
         <v>6.24</v>
       </c>
-      <c r="AD9" t="n">
+      <c r="AI9" t="n">
         <v>23.42</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AJ9" t="n">
         <v>13.79</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AK9" t="n">
         <v>34.62</v>
       </c>
-      <c r="AG9" t="n">
+      <c r="AL9" t="n">
         <v>-10.84</v>
       </c>
     </row>
@@ -1426,93 +1538,108 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-0.16</v>
+        <v>2.87</v>
       </c>
       <c r="E10" t="n">
+        <v>-0.17</v>
+      </c>
+      <c r="F10" t="n">
         <v>-0.06</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>-0.13</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>-0.06</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>-0.15</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>0.04</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
+        <v>-3.21</v>
+      </c>
+      <c r="L10" t="n">
         <v>2.08</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>0.02</v>
       </c>
-      <c r="L10" t="n">
+      <c r="N10" t="n">
         <v>0.14</v>
       </c>
-      <c r="M10" t="n">
+      <c r="O10" t="n">
         <v>-0.02</v>
       </c>
-      <c r="N10" t="n">
+      <c r="P10" t="n">
         <v>0.03</v>
       </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
         <v>-0.27</v>
       </c>
-      <c r="P10" t="n">
+      <c r="R10" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="S10" t="n">
         <v>-6.92</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="T10" t="n">
         <v>-0.03</v>
       </c>
-      <c r="R10" t="n">
+      <c r="U10" t="n">
         <v>-0.41</v>
       </c>
-      <c r="S10" t="n">
+      <c r="V10" t="n">
         <v>-0.04</v>
       </c>
-      <c r="T10" t="n">
+      <c r="W10" t="n">
         <v>-0.24</v>
       </c>
-      <c r="U10" t="n">
+      <c r="X10" t="n">
         <v>0.74</v>
       </c>
-      <c r="V10" t="n">
+      <c r="Y10" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Z10" t="n">
         <v>-1.16</v>
       </c>
-      <c r="W10" t="n">
+      <c r="AA10" t="n">
         <v>0.65</v>
       </c>
-      <c r="X10" t="n">
+      <c r="AB10" t="n">
         <v>0.17</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="AC10" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AD10" t="n">
         <v>-0.22</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AE10" t="n">
         <v>0.76</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AF10" t="n">
+        <v>351.92</v>
+      </c>
+      <c r="AG10" t="n">
         <v>20.18</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AH10" t="n">
         <v>8.17</v>
       </c>
-      <c r="AD10" t="n">
+      <c r="AI10" t="n">
         <v>20.11</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AJ10" t="n">
         <v>9.92</v>
       </c>
-      <c r="AF10" t="n">
+      <c r="AK10" t="n">
         <v>26.49</v>
       </c>
-      <c r="AG10" t="n">
+      <c r="AL10" t="n">
         <v>-8.06</v>
       </c>
     </row>
@@ -1525,93 +1652,108 @@
         </is>
       </c>
       <c r="D11" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E11" t="n">
         <v>-0.09</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>-0.03</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>-0.09</v>
       </c>
-      <c r="G11" t="n">
-        <v>-0.1</v>
-      </c>
       <c r="H11" t="n">
-        <v>-0.18</v>
+        <v>-0.11</v>
       </c>
       <c r="I11" t="n">
+        <v>-0.17</v>
+      </c>
+      <c r="J11" t="n">
         <v>0.04</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
+        <v>-1.16</v>
+      </c>
+      <c r="L11" t="n">
         <v>0.68</v>
       </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
         <v>0.14</v>
       </c>
-      <c r="L11" t="n">
+      <c r="N11" t="n">
         <v>-0.32</v>
       </c>
-      <c r="M11" t="n">
+      <c r="O11" t="n">
         <v>-0.01</v>
       </c>
-      <c r="N11" t="n">
+      <c r="P11" t="n">
         <v>0.17</v>
       </c>
-      <c r="O11" t="n">
+      <c r="Q11" t="n">
         <v>-0.82</v>
       </c>
-      <c r="P11" t="n">
+      <c r="R11" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="S11" t="n">
         <v>-1.68</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="T11" t="n">
         <v>-0.33</v>
       </c>
-      <c r="R11" t="n">
+      <c r="U11" t="n">
         <v>0.68</v>
       </c>
-      <c r="S11" t="n">
+      <c r="V11" t="n">
         <v>-0.09</v>
       </c>
-      <c r="T11" t="n">
+      <c r="W11" t="n">
         <v>-0.47</v>
       </c>
-      <c r="U11" t="n">
+      <c r="X11" t="n">
         <v>1.65</v>
       </c>
-      <c r="V11" t="n">
+      <c r="Y11" t="n">
+        <v>10.79</v>
+      </c>
+      <c r="Z11" t="n">
         <v>-3.54</v>
       </c>
-      <c r="W11" t="n">
+      <c r="AA11" t="n">
         <v>-1.72</v>
       </c>
-      <c r="X11" t="n">
+      <c r="AB11" t="n">
         <v>-1.18</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AC11" t="n">
         <v>-0.8100000000000001</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AD11" t="n">
         <v>-1.34</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AE11" t="n">
         <v>0.34</v>
       </c>
-      <c r="AB11" t="n">
+      <c r="AF11" t="n">
+        <v>417.11</v>
+      </c>
+      <c r="AG11" t="n">
         <v>17.1</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AH11" t="n">
         <v>6.41</v>
       </c>
-      <c r="AD11" t="n">
+      <c r="AI11" t="n">
         <v>18.5</v>
       </c>
-      <c r="AE11" t="n">
+      <c r="AJ11" t="n">
         <v>23.25</v>
       </c>
-      <c r="AF11" t="n">
+      <c r="AK11" t="n">
         <v>44.4</v>
       </c>
-      <c r="AG11" t="n">
+      <c r="AL11" t="n">
         <v>-9.75</v>
       </c>
     </row>
@@ -1628,93 +1770,108 @@
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="E12" t="n">
         <v>-0.12</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>-0.2</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>-0.08</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>-0.01</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>-0.31</v>
       </c>
-      <c r="I12" t="n">
-        <v>0.05</v>
-      </c>
       <c r="J12" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K12" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="L12" t="n">
         <v>-5.51</v>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>-0.42</v>
       </c>
-      <c r="L12" t="n">
+      <c r="N12" t="n">
         <v>0.06</v>
       </c>
-      <c r="M12" t="n">
+      <c r="O12" t="n">
         <v>-0.04</v>
       </c>
-      <c r="N12" t="n">
+      <c r="P12" t="n">
         <v>0</v>
       </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
         <v>-0.24</v>
       </c>
-      <c r="P12" t="n">
+      <c r="R12" t="n">
+        <v>-30.13</v>
+      </c>
+      <c r="S12" t="n">
         <v>29.59</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="T12" t="n">
         <v>2.16</v>
       </c>
-      <c r="R12" t="n">
+      <c r="U12" t="n">
         <v>-0.34</v>
       </c>
-      <c r="S12" t="n">
+      <c r="V12" t="n">
         <v>0.23</v>
       </c>
-      <c r="T12" t="n">
+      <c r="W12" t="n">
         <v>-0.07000000000000001</v>
       </c>
-      <c r="U12" t="n">
+      <c r="X12" t="n">
         <v>1.16</v>
       </c>
-      <c r="V12" t="n">
+      <c r="Y12" t="n">
+        <v>-9.92</v>
+      </c>
+      <c r="Z12" t="n">
         <v>-5.48</v>
       </c>
-      <c r="W12" t="n">
+      <c r="AA12" t="n">
         <v>2.99</v>
       </c>
-      <c r="X12" t="n">
+      <c r="AB12" t="n">
         <v>1.68</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AC12" t="n">
         <v>1.23</v>
       </c>
-      <c r="Z12" t="n">
+      <c r="AD12" t="n">
         <v>1.63</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AE12" t="n">
         <v>2.97</v>
       </c>
-      <c r="AB12" t="n">
+      <c r="AF12" t="n">
+        <v>184.7</v>
+      </c>
+      <c r="AG12" t="n">
         <v>4.42</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AH12" t="n">
         <v>7.32</v>
       </c>
-      <c r="AD12" t="n">
+      <c r="AI12" t="n">
         <v>3.14</v>
       </c>
-      <c r="AE12" t="n">
+      <c r="AJ12" t="n">
         <v>0.13</v>
       </c>
-      <c r="AF12" t="n">
+      <c r="AK12" t="n">
         <v>13.35</v>
       </c>
-      <c r="AG12" t="n">
+      <c r="AL12" t="n">
         <v>-2.33</v>
       </c>
     </row>
@@ -1727,93 +1884,108 @@
         </is>
       </c>
       <c r="D13" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E13" t="n">
         <v>2.07</v>
       </c>
-      <c r="E13" t="n">
-        <v>-0.21</v>
-      </c>
       <c r="F13" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="G13" t="n">
         <v>-0.39</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>-0.06</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>-0.12</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>0.02</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
+        <v>-66.63</v>
+      </c>
+      <c r="L13" t="n">
         <v>63.19</v>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>1.44</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>1.32</v>
       </c>
-      <c r="M13" t="n">
+      <c r="O13" t="n">
         <v>0</v>
       </c>
-      <c r="N13" t="n">
+      <c r="P13" t="n">
         <v>0.19</v>
       </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
         <v>0.05</v>
       </c>
-      <c r="P13" t="n">
+      <c r="R13" t="n">
+        <v>-8.84</v>
+      </c>
+      <c r="S13" t="n">
         <v>24.31</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="T13" t="n">
         <v>-6.56</v>
       </c>
-      <c r="R13" t="n">
+      <c r="U13" t="n">
         <v>-6.22</v>
       </c>
-      <c r="S13" t="n">
+      <c r="V13" t="n">
         <v>0.02</v>
       </c>
-      <c r="T13" t="n">
+      <c r="W13" t="n">
         <v>-0.7</v>
       </c>
-      <c r="U13" t="n">
+      <c r="X13" t="n">
         <v>-0.28</v>
       </c>
-      <c r="V13" t="n">
+      <c r="Y13" t="n">
+        <v>-4.98</v>
+      </c>
+      <c r="Z13" t="n">
         <v>-9.82</v>
       </c>
-      <c r="W13" t="n">
+      <c r="AA13" t="n">
         <v>7.8</v>
       </c>
-      <c r="X13" t="n">
+      <c r="AB13" t="n">
         <v>0.66</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="AC13" t="n">
         <v>2.09</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="AD13" t="n">
         <v>0.67</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AE13" t="n">
         <v>1.6</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AF13" t="n">
+        <v>13710.22</v>
+      </c>
+      <c r="AG13" t="n">
         <v>-13506.22</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AH13" t="n">
         <v>8.98</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AI13" t="n">
         <v>18.74</v>
       </c>
-      <c r="AE13" t="n">
+      <c r="AJ13" t="n">
         <v>4.6</v>
       </c>
-      <c r="AF13" t="n">
+      <c r="AK13" t="n">
         <v>5.6</v>
       </c>
-      <c r="AG13" t="n">
+      <c r="AL13" t="n">
         <v>-2.02</v>
       </c>
     </row>
@@ -1830,93 +2002,108 @@
         </is>
       </c>
       <c r="D14" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="E14" t="n">
         <v>-0.33</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>-0.23</v>
       </c>
-      <c r="F14" t="n">
-        <v>-0.41</v>
-      </c>
       <c r="G14" t="n">
+        <v>-0.42</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.03</v>
       </c>
-      <c r="H14" t="n">
-        <v>-0.17</v>
-      </c>
       <c r="I14" t="n">
-        <v>0.07000000000000001</v>
+        <v>-0.18</v>
       </c>
       <c r="J14" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-3.98</v>
+      </c>
+      <c r="L14" t="n">
         <v>3.64</v>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>-0.01</v>
       </c>
-      <c r="L14" t="n">
+      <c r="N14" t="n">
         <v>0.6</v>
       </c>
-      <c r="M14" t="n">
+      <c r="O14" t="n">
         <v>-0.29</v>
       </c>
-      <c r="N14" t="n">
+      <c r="P14" t="n">
         <v>0.08</v>
       </c>
-      <c r="O14" t="n">
+      <c r="Q14" t="n">
         <v>-0.49</v>
       </c>
-      <c r="P14" t="n">
+      <c r="R14" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="S14" t="n">
         <v>-22.04</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="T14" t="n">
         <v>-0.02</v>
       </c>
-      <c r="R14" t="n">
+      <c r="U14" t="n">
         <v>-2.78</v>
       </c>
-      <c r="S14" t="n">
+      <c r="V14" t="n">
         <v>1.32</v>
       </c>
-      <c r="T14" t="n">
+      <c r="W14" t="n">
         <v>-0.4</v>
       </c>
-      <c r="U14" t="n">
+      <c r="X14" t="n">
         <v>2.27</v>
       </c>
-      <c r="V14" t="n">
+      <c r="Y14" t="n">
+        <v>-1.36</v>
+      </c>
+      <c r="Z14" t="n">
         <v>-1.7</v>
       </c>
-      <c r="W14" t="n">
+      <c r="AA14" t="n">
         <v>2.04</v>
       </c>
-      <c r="X14" t="n">
+      <c r="AB14" t="n">
         <v>-1.51</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AC14" t="n">
         <v>1.68</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="AD14" t="n">
         <v>-0.19</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AE14" t="n">
         <v>2.66</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AF14" t="n">
+        <v>186.91</v>
+      </c>
+      <c r="AG14" t="n">
         <v>11.8</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AH14" t="n">
         <v>9.369999999999999</v>
       </c>
-      <c r="AD14" t="n">
+      <c r="AI14" t="n">
         <v>19.21</v>
       </c>
-      <c r="AE14" t="n">
+      <c r="AJ14" t="n">
         <v>-1.34</v>
       </c>
-      <c r="AF14" t="n">
+      <c r="AK14" t="n">
         <v>9.16</v>
       </c>
-      <c r="AG14" t="n">
+      <c r="AL14" t="n">
         <v>-3.68</v>
       </c>
     </row>
@@ -1929,110 +2116,127 @@
         </is>
       </c>
       <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="n">
         <v>-0.41</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>-0.11</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>-0.35</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>-0.17</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>-0.07000000000000001</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>0.01</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="L15" t="n">
         <v>3.8</v>
       </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
         <v>0</v>
       </c>
-      <c r="L15" t="n">
+      <c r="N15" t="n">
         <v>0.2</v>
       </c>
-      <c r="M15" t="n">
+      <c r="O15" t="n">
         <v>0.28</v>
       </c>
-      <c r="N15" t="n">
+      <c r="P15" t="n">
         <v>0.02</v>
       </c>
-      <c r="O15" t="n">
+      <c r="Q15" t="n">
         <v>-0.73</v>
       </c>
-      <c r="P15" t="n">
+      <c r="R15" t="n">
+        <v>18.54</v>
+      </c>
+      <c r="S15" t="n">
         <v>-18.92</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="T15" t="n">
         <v>-0.01</v>
       </c>
-      <c r="R15" t="n">
+      <c r="U15" t="n">
         <v>-0.8</v>
       </c>
-      <c r="S15" t="n">
+      <c r="V15" t="n">
         <v>-1.06</v>
       </c>
-      <c r="T15" t="n">
+      <c r="W15" t="n">
         <v>-0.2</v>
       </c>
-      <c r="U15" t="n">
+      <c r="X15" t="n">
         <v>2.95</v>
       </c>
-      <c r="V15" t="n">
+      <c r="Y15" t="n">
+        <v>11.22</v>
+      </c>
+      <c r="Z15" t="n">
         <v>-6.16</v>
       </c>
-      <c r="W15" t="n">
+      <c r="AA15" t="n">
         <v>-0.17</v>
       </c>
-      <c r="X15" t="n">
+      <c r="AB15" t="n">
         <v>-2.08</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AC15" t="n">
         <v>-1.64</v>
       </c>
-      <c r="Z15" t="n">
+      <c r="AD15" t="n">
         <v>-0.74</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AE15" t="n">
         <v>1.5</v>
       </c>
-      <c r="AB15" t="n">
+      <c r="AF15" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="AG15" t="n">
         <v>17.8</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AH15" t="n">
         <v>5.34</v>
       </c>
-      <c r="AD15" t="n">
+      <c r="AI15" t="n">
         <v>19</v>
       </c>
-      <c r="AE15" t="n">
+      <c r="AJ15" t="n">
         <v>10.33</v>
       </c>
-      <c r="AF15" t="n">
+      <c r="AK15" t="n">
         <v>4.44</v>
       </c>
-      <c r="AG15" t="n">
+      <c r="AL15" t="n">
         <v>-0.71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="Y1:AE1"/>
     <mergeCell ref="A4:A7"/>
-    <mergeCell ref="V1:AA1"/>
-    <mergeCell ref="AB1:AG1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="B12:B13"/>
+    <mergeCell ref="R1:X1"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B8:B9"/>
+    <mergeCell ref="AF1:AL1"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="K1:Q1"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D1:J1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2061,7 +2265,7 @@
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="13.2" customWidth="1" min="9" max="9"/>
-    <col width="18" customWidth="1" min="10" max="10"/>
+    <col width="25.2" customWidth="1" min="10" max="10"/>
     <col width="22.8" customWidth="1" min="11" max="11"/>
     <col width="27.6" customWidth="1" min="12" max="12"/>
     <col width="22.8" customWidth="1" min="13" max="13"/>
@@ -2515,176 +2719,168 @@
           <t>ctrl</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>vx770</t>
-        </is>
-      </c>
+      <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.13</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="T4" t="n">
         <v>0.01</v>
       </c>
-      <c r="I4" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="J4" t="n">
-        <v>-0.21</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="Y4" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="AD4" t="n">
         <v>-0.27</v>
       </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>22.92</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1.32</v>
-      </c>
       <c r="AE4" t="n">
-        <v>-7.01</v>
+        <v>-1.71</v>
       </c>
       <c r="AJ4" t="n">
-        <v>-9.82</v>
+        <v>-0.6699999999999999</v>
       </c>
       <c r="AO4" t="n">
-        <v>6.38</v>
+        <v>-2.21</v>
       </c>
       <c r="AT4" t="n">
-        <v>19.76</v>
+        <v>-0.16</v>
       </c>
       <c r="AY4" t="n">
-        <v>20.58</v>
+        <v>0.26</v>
       </c>
       <c r="AZ4" t="n">
-        <v>31.19</v>
+        <v>-0.52</v>
       </c>
       <c r="BE4" t="n">
-        <v>38.33</v>
+        <v>-0.04000000000000004</v>
       </c>
       <c r="BJ4" t="n">
-        <v>13.66</v>
+        <v>-1.43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="n"/>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>vx661-vx445</t>
-        </is>
-      </c>
+      <c r="B5" s="10" t="n"/>
       <c r="C5" s="1" t="inlineStr">
         <is>
           <t>vx770</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.05</v>
+        <v>-0.08</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.18</v>
+        <v>-0.21</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.24</v>
+        <v>-0.27</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>-2.51</v>
+        <v>22.92</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.73</v>
+        <v>1.32</v>
       </c>
       <c r="AE5" t="n">
-        <v>-3.71</v>
+        <v>-7.01</v>
       </c>
       <c r="AJ5" t="n">
-        <v>-4.74</v>
+        <v>-9.82</v>
       </c>
       <c r="AO5" t="n">
-        <v>-0.11</v>
+        <v>6.38</v>
       </c>
       <c r="AT5" t="n">
-        <v>7.33</v>
+        <v>19.76</v>
       </c>
       <c r="AY5" t="n">
-        <v>6.24</v>
+        <v>20.58</v>
       </c>
       <c r="AZ5" t="n">
-        <v>8.460000000000001</v>
+        <v>31.19</v>
       </c>
       <c r="BE5" t="n">
-        <v>9.380000000000001</v>
+        <v>38.33</v>
       </c>
       <c r="BJ5" t="n">
-        <v>1.1</v>
+        <v>13.66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>ctrl</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr"/>
+          <t>vx661-vx445</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>vx770</t>
+        </is>
+      </c>
       <c r="D6" t="n">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="I6" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="T6" t="n">
         <v>-0.04</v>
       </c>
-      <c r="J6" t="n">
-        <v>-0.27</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="T6" t="n">
-        <v>-0.06</v>
-      </c>
       <c r="Y6" t="n">
-        <v>30.17</v>
+        <v>-2.51</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.53</v>
+        <v>-0.73</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.02000000000000002</v>
+        <v>-3.71</v>
       </c>
       <c r="AJ6" t="n">
-        <v>-0.39</v>
+        <v>-4.74</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.79</v>
+        <v>-0.11</v>
       </c>
       <c r="AT6" t="n">
-        <v>-0.93</v>
+        <v>7.33</v>
       </c>
       <c r="AY6" t="n">
-        <v>2.08</v>
+        <v>6.24</v>
       </c>
       <c r="AZ6" t="n">
-        <v>2.68</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="BE6" t="n">
-        <v>3.26</v>
+        <v>9.380000000000001</v>
       </c>
       <c r="BJ6" t="n">
-        <v>1.64</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n"/>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>vx661-vx445</t>
-        </is>
-      </c>
+      <c r="B7" s="10" t="n"/>
       <c r="C7" s="1" t="inlineStr">
         <is>
           <t>vx770-Api</t>
@@ -2755,10 +2951,10 @@
         <v>-0.04</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.11</v>
+        <v>-0.1</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.15</v>
+        <v>-0.14</v>
       </c>
       <c r="T8" t="n">
         <v>-0.15</v>
@@ -2861,7 +3057,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="I10" t="n">
         <v>-0.06</v>
@@ -2924,10 +3120,10 @@
         <v>-0.12</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.18</v>
+        <v>-0.17</v>
       </c>
       <c r="Y11" t="n">
         <v>-1.68</v>
@@ -3030,13 +3226,13 @@
         <v>2.07</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.21</v>
+        <v>-0.2</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.6</v>
+        <v>-0.5900000000000001</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.6599999999999999</v>
+        <v>-0.6500000000000001</v>
       </c>
       <c r="T13" t="n">
         <v>-0.12</v>
@@ -3091,13 +3287,13 @@
         <v>-0.23</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.64</v>
+        <v>-0.65</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.61</v>
+        <v>-0.62</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="Y14" t="n">
         <v>-22.04</v>
@@ -3185,8 +3381,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="D1:X1"/>
@@ -3195,6 +3392,7 @@
     <mergeCell ref="Y1:AS1"/>
     <mergeCell ref="AT1:BN1"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>